<commit_message>
pipeline: Add new field to spreadsheets
    service_and_beneficiaries / country_classification
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/pipeline_public_v001.xlsx
+++ b/indigo/spreadsheetform_guides/pipeline_public_v001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="665">
   <si>
     <t xml:space="preserve">INDIGO Pipeline ID</t>
   </si>
@@ -553,6 +553,33 @@
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:SINGLE:service_and_beneficiaries/unit_description_of_service_user_or_beneficiaries/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country Classification of Service and beneficiaries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low-income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:service_and_beneficiaries/country_classification/low_income/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lower-middle-income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:service_and_beneficiaries/country_classification/lower_middle_income/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upper-middle-income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:service_and_beneficiaries/country_classification/upper_middle_income/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High-income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:service_and_beneficiaries/country_classification/high_income/value</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:SINGLE:service_and_beneficiaries/source_ids</t>
@@ -2343,7 +2370,7 @@
   </sheetPr>
   <dimension ref="A2:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2411,47 +2438,47 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -2494,22 +2521,22 @@
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="E2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>21</v>
@@ -2517,19 +2544,19 @@
     </row>
     <row r="4" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2805,58 +2832,58 @@
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="Q2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>21</v>
@@ -2864,55 +2891,55 @@
     </row>
     <row r="4" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3502,277 +3529,277 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -3808,15 +3835,15 @@
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>21</v>
@@ -3824,13 +3851,13 @@
     </row>
     <row r="4" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4002,1247 +4029,1247 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>425</v>
+        <v>434</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>438</v>
+        <v>447</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>441</v>
+        <v>450</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>445</v>
+        <v>454</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>446</v>
+        <v>455</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>448</v>
+        <v>457</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>450</v>
+        <v>459</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>452</v>
+        <v>461</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>453</v>
+        <v>462</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>455</v>
+        <v>464</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>456</v>
+        <v>465</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>457</v>
+        <v>466</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>458</v>
+        <v>467</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>459</v>
+        <v>468</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>467</v>
+        <v>476</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>468</v>
+        <v>477</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>469</v>
+        <v>478</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>470</v>
+        <v>479</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>471</v>
+        <v>480</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>472</v>
+        <v>481</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>473</v>
+        <v>482</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>474</v>
+        <v>483</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>475</v>
+        <v>484</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>477</v>
+        <v>486</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>478</v>
+        <v>487</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>479</v>
+        <v>488</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>480</v>
+        <v>489</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>481</v>
+        <v>490</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>482</v>
+        <v>491</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>484</v>
+        <v>493</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>485</v>
+        <v>494</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>486</v>
+        <v>495</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>487</v>
+        <v>496</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>488</v>
+        <v>497</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>489</v>
+        <v>498</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>490</v>
+        <v>499</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>491</v>
+        <v>500</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>492</v>
+        <v>501</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>493</v>
+        <v>502</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>494</v>
+        <v>503</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>495</v>
+        <v>504</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>496</v>
+        <v>505</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>497</v>
+        <v>506</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>498</v>
+        <v>507</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>499</v>
+        <v>508</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>500</v>
+        <v>509</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>501</v>
+        <v>510</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>502</v>
+        <v>511</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>503</v>
+        <v>512</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>504</v>
+        <v>513</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>505</v>
+        <v>514</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>506</v>
+        <v>515</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>507</v>
+        <v>516</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>508</v>
+        <v>517</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>509</v>
+        <v>518</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>510</v>
+        <v>519</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>511</v>
+        <v>520</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>512</v>
+        <v>521</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>513</v>
+        <v>522</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>514</v>
+        <v>523</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>515</v>
+        <v>524</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>516</v>
+        <v>525</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>517</v>
+        <v>526</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>518</v>
+        <v>527</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>519</v>
+        <v>528</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>520</v>
+        <v>529</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>521</v>
+        <v>530</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>522</v>
+        <v>531</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>523</v>
+        <v>532</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>524</v>
+        <v>533</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>525</v>
+        <v>534</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>526</v>
+        <v>535</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>527</v>
+        <v>536</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>528</v>
+        <v>537</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>529</v>
+        <v>538</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>530</v>
+        <v>539</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>531</v>
+        <v>540</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>532</v>
+        <v>541</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>533</v>
+        <v>542</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>534</v>
+        <v>543</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>535</v>
+        <v>544</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>536</v>
+        <v>545</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>537</v>
+        <v>546</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>538</v>
+        <v>547</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>539</v>
+        <v>548</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>540</v>
+        <v>549</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>541</v>
+        <v>550</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>542</v>
+        <v>551</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>543</v>
+        <v>552</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>544</v>
+        <v>553</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>545</v>
+        <v>554</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>546</v>
+        <v>555</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>547</v>
+        <v>556</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>548</v>
+        <v>557</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>549</v>
+        <v>558</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>550</v>
+        <v>559</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>552</v>
+        <v>561</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>553</v>
+        <v>562</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>554</v>
+        <v>563</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>555</v>
+        <v>564</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>556</v>
+        <v>565</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>557</v>
+        <v>566</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>558</v>
+        <v>567</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>559</v>
+        <v>568</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>560</v>
+        <v>569</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>561</v>
+        <v>570</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>562</v>
+        <v>571</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>563</v>
+        <v>572</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>564</v>
+        <v>573</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>565</v>
+        <v>574</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>566</v>
+        <v>575</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>567</v>
+        <v>576</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>568</v>
+        <v>577</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>569</v>
+        <v>578</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>570</v>
+        <v>579</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>571</v>
+        <v>580</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>572</v>
+        <v>581</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>573</v>
+        <v>582</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>574</v>
+        <v>583</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>575</v>
+        <v>584</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>576</v>
+        <v>585</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>577</v>
+        <v>586</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>578</v>
+        <v>587</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>579</v>
+        <v>588</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>580</v>
+        <v>589</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>581</v>
+        <v>590</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>582</v>
+        <v>591</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>583</v>
+        <v>592</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>584</v>
+        <v>593</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>585</v>
+        <v>594</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>586</v>
+        <v>595</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>587</v>
+        <v>596</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>588</v>
+        <v>597</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>589</v>
+        <v>598</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>590</v>
+        <v>599</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>591</v>
+        <v>600</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>592</v>
+        <v>601</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>593</v>
+        <v>602</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>594</v>
+        <v>603</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>595</v>
+        <v>604</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>596</v>
+        <v>605</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>597</v>
+        <v>606</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>598</v>
+        <v>607</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>599</v>
+        <v>608</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>600</v>
+        <v>609</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>601</v>
+        <v>610</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>602</v>
+        <v>611</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>603</v>
+        <v>612</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>604</v>
+        <v>613</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>605</v>
+        <v>614</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>606</v>
+        <v>615</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>607</v>
+        <v>616</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>608</v>
+        <v>617</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>609</v>
+        <v>618</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>610</v>
+        <v>619</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>611</v>
+        <v>620</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>612</v>
+        <v>621</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>613</v>
+        <v>622</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>614</v>
+        <v>623</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>615</v>
+        <v>624</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>616</v>
+        <v>625</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>617</v>
+        <v>626</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>618</v>
+        <v>627</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>619</v>
+        <v>628</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>621</v>
+        <v>630</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>622</v>
+        <v>631</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>623</v>
+        <v>632</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>624</v>
+        <v>633</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>625</v>
+        <v>634</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>626</v>
+        <v>635</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>627</v>
+        <v>636</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>628</v>
+        <v>637</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>629</v>
+        <v>638</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>630</v>
+        <v>639</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>631</v>
+        <v>640</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>632</v>
+        <v>641</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>633</v>
+        <v>642</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>634</v>
+        <v>643</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>636</v>
+        <v>645</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>637</v>
+        <v>646</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>639</v>
+        <v>648</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>640</v>
+        <v>649</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>641</v>
+        <v>650</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>643</v>
+        <v>652</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>644</v>
+        <v>653</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>645</v>
+        <v>654</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>646</v>
+        <v>655</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>647</v>
+        <v>656</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>648</v>
+        <v>657</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>649</v>
+        <v>658</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>650</v>
+        <v>659</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>651</v>
+        <v>660</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>652</v>
+        <v>661</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>653</v>
+        <v>662</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>654</v>
+        <v>663</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>655</v>
+        <v>664</v>
       </c>
     </row>
   </sheetData>
@@ -5261,9 +5288,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:G133"/>
+  <dimension ref="A2:G137"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6303,35 +6330,73 @@
         <v>170</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="4" t="s">
+    <row r="130" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="8"/>
+      <c r="B131" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C131" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="8"/>
+      <c r="B132" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="8"/>
+      <c r="B133" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B130" s="4"/>
-      <c r="C130" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="4" t="s">
+      <c r="B134" s="4"/>
+      <c r="C134" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B131" s="4"/>
-      <c r="C131" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="4" t="s">
+      <c r="B135" s="4"/>
+      <c r="C135" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B133" s="5"/>
-      <c r="C133" s="6" t="s">
-        <v>173</v>
+      <c r="B137" s="5"/>
+      <c r="C137" s="6" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="15">
+  <dataValidations count="16">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C128" type="list">
       <formula1>"Individual,Other"</formula1>
       <formula2>0</formula2>
@@ -6392,6 +6457,10 @@
       <formula1>"0-6 months,6-12 months,12-24 months,&gt;24 months "</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C130:C133" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D118" r:id="rId1" display="https://github.com/datapopalliance/SDGs/blob/master/SDG-goals.csv "/>
@@ -6426,16 +6495,16 @@
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13"/>
       <c r="B3" s="4" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -6443,13 +6512,13 @@
     </row>
     <row r="5" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6546,34 +6615,34 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="15" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6581,7 +6650,7 @@
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -6594,34 +6663,34 @@
     </row>
     <row r="4" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7007,54 +7076,54 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13"/>
       <c r="B2" s="4" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="K2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>21</v>
@@ -7062,37 +7131,37 @@
     </row>
     <row r="4" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7500,11 +7569,11 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -7525,10 +7594,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>40</v>
@@ -7540,51 +7609,51 @@
         <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7998,35 +8067,35 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="H2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>124</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>21</v>
@@ -8034,28 +8103,28 @@
     </row>
     <row r="4" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8394,7 +8463,7 @@
       <c r="A2" s="13"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -8402,51 +8471,51 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="M2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>21</v>
@@ -8454,43 +8523,43 @@
     </row>
     <row r="4" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8976,7 +9045,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="11"/>
       <c r="K2" s="0" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="L2" s="11"/>
       <c r="N2" s="11"/>
@@ -8987,7 +9056,7 @@
       <c r="B3" s="13"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -8996,67 +9065,67 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="Q3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="P4" s="13" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="Q4" s="4" t="s">
         <v>21</v>
@@ -9064,55 +9133,55 @@
     </row>
     <row r="5" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
pipeline: Add organisation names to public spreadsheet
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/pipeline_public_v001.xlsx
+++ b/indigo/spreadsheetform_guides/pipeline_public_v001.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="669">
   <si>
     <t xml:space="preserve">INDIGO Pipeline ID</t>
   </si>
@@ -777,13 +777,13 @@
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:organisations:country/value</t>
   </si>
   <si>
+    <t xml:space="preserve">Organisation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Planned Service</t>
   </si>
   <si>
     <t xml:space="preserve">Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organisation ID</t>
   </si>
   <si>
     <t xml:space="preserve">Organisation 
@@ -802,6 +802,9 @@
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:service_provisions:organisation_id/value</t>
   </si>
   <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:service_provisions:organisation_names/organisation_id/value</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:service_provisions:organisation_role_category/value</t>
   </si>
   <si>
@@ -845,6 +848,9 @@
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_payment_commitments:organisation_id/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_payment_commitments:organisation_names/organisation_id/value</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_payment_commitments:organisation_role_category/value</t>
@@ -936,6 +942,9 @@
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:investments:organisation_id/value</t>
   </si>
   <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:investments:organisation_names/organisation_id/value</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:investments:organisation_role_category/value</t>
   </si>
   <si>
@@ -1013,6 +1022,9 @@
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:intermediary_services:organisation_id/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:intermediary_services:organisation_names/organisation_id/value</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:intermediary_services:organisation_role_category/value</t>
@@ -2111,7 +2123,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2121,13 +2133,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEF413D"/>
-        <bgColor rgb="FF993366"/>
+        <bgColor rgb="FFED1C24"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFCD3C1"/>
-        <bgColor rgb="FFFEDCC6"/>
+        <bgColor rgb="FFFCD4D1"/>
       </patternFill>
     </fill>
     <fill>
@@ -2168,8 +2180,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFED1C24"/>
+        <bgColor rgb="FFEF413D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFE0EFD4"/>
         <bgColor rgb="FFE7E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCD4D1"/>
+        <bgColor rgb="FFFCD3C1"/>
       </patternFill>
     </fill>
   </fills>
@@ -2214,7 +2238,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2287,7 +2311,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2304,7 +2336,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFED1C24"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -2325,7 +2357,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFFCD4D1"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -2438,47 +2470,47 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -2497,7 +2529,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -2506,261 +2538,298 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" s="13"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="B3" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="101.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>322</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>323</v>
+        <v>325</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>326</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>325</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14"/>
-      <c r="B5" s="6"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14"/>
-      <c r="B6" s="6"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14"/>
-      <c r="B7" s="6"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="14"/>
-      <c r="B8" s="6"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14"/>
-      <c r="B9" s="6"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14"/>
-      <c r="B10" s="6"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14"/>
-      <c r="B11" s="6"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14"/>
-      <c r="B12" s="6"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="14"/>
-      <c r="B13" s="6"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14"/>
-      <c r="B14" s="6"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="14"/>
-      <c r="B15" s="6"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="14"/>
-      <c r="B16" s="6"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="14"/>
-      <c r="B17" s="6"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="14"/>
-      <c r="B18" s="6"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="14"/>
-      <c r="B19" s="6"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="14"/>
-      <c r="B20" s="6"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14"/>
-      <c r="B21" s="6"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14"/>
-      <c r="B22" s="6"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14"/>
-      <c r="B23" s="6"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="14"/>
-      <c r="B24" s="6"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="14"/>
-      <c r="B25" s="6"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="14"/>
-      <c r="B26" s="6"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="14"/>
-      <c r="B27" s="6"/>
+      <c r="B27" s="20"/>
       <c r="C27" s="6"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="14"/>
-      <c r="B28" s="6"/>
+      <c r="B28" s="20"/>
       <c r="C28" s="6"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="14"/>
-      <c r="B29" s="6"/>
+      <c r="B29" s="20"/>
       <c r="C29" s="6"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="14"/>
-      <c r="B30" s="6"/>
+      <c r="B30" s="20"/>
       <c r="C30" s="6"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="14"/>
-      <c r="B31" s="6"/>
+      <c r="B31" s="20"/>
       <c r="C31" s="6"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="14"/>
-      <c r="B32" s="6"/>
+      <c r="B32" s="20"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B4:B32" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C4:C32" type="list">
       <formula1>"Impact bond design,Financial and commercial modeling,Impact bond investment structure,Capital raise ,Loan arranger,Performance management,Legal counsel,Technical assistance,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2783,7 +2852,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2838,49 +2907,49 @@
     </row>
     <row r="3" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="P3" s="13" t="s">
         <v>185</v>
@@ -2890,60 +2959,60 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
-        <v>341</v>
+      <c r="A4" s="19" t="s">
+        <v>345</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -2962,7 +3031,7 @@
       <c r="Q5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -2981,7 +3050,7 @@
       <c r="Q6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -3000,7 +3069,7 @@
       <c r="Q7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -3019,7 +3088,7 @@
       <c r="Q8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -3038,7 +3107,7 @@
       <c r="Q9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -3057,7 +3126,7 @@
       <c r="Q10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -3076,7 +3145,7 @@
       <c r="Q11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -3095,7 +3164,7 @@
       <c r="Q12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -3114,7 +3183,7 @@
       <c r="Q13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -3133,7 +3202,7 @@
       <c r="Q14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -3152,7 +3221,7 @@
       <c r="Q15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="18"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -3171,7 +3240,7 @@
       <c r="Q16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -3190,7 +3259,7 @@
       <c r="Q17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -3209,7 +3278,7 @@
       <c r="Q18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="18"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -3228,7 +3297,7 @@
       <c r="Q19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="18"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -3247,7 +3316,7 @@
       <c r="Q20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -3266,7 +3335,7 @@
       <c r="Q21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="18"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -3285,7 +3354,7 @@
       <c r="Q22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -3304,7 +3373,7 @@
       <c r="Q23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="18"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -3323,7 +3392,7 @@
       <c r="Q24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="18"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -3342,7 +3411,7 @@
       <c r="Q25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="18"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -3361,7 +3430,7 @@
       <c r="Q26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="18"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -3380,7 +3449,7 @@
       <c r="Q27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="18"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -3399,7 +3468,7 @@
       <c r="Q28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="18"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -3418,7 +3487,7 @@
       <c r="Q29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="18"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -3437,7 +3506,7 @@
       <c r="Q30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="18"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -3456,7 +3525,7 @@
       <c r="Q31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="18"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -3529,277 +3598,277 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -3840,7 +3909,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>192</v>
@@ -3851,13 +3920,13 @@
     </row>
     <row r="4" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4029,502 +4098,502 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4534,742 +4603,742 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>587</v>
+        <v>591</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>608</v>
+        <v>612</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>637</v>
+        <v>641</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>653</v>
+        <v>657</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>655</v>
+        <v>659</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>657</v>
+        <v>661</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>660</v>
+        <v>664</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>662</v>
+        <v>666</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>663</v>
+        <v>667</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>664</v>
+        <v>668</v>
       </c>
     </row>
   </sheetData>
@@ -8041,7 +8110,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -8051,64 +8120,70 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.19"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.19"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="15"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" s="13"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
+    <row r="4" customFormat="false" ht="115.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="19" t="s">
         <v>251</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="20" t="s">
         <v>253</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -8120,300 +8195,331 @@
       <c r="F4" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="14" t="s">
         <v>258</v>
       </c>
+      <c r="I4" s="6" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="14"/>
-      <c r="C5" s="6"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="14"/>
-      <c r="C6" s="6"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="6"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="6"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="14"/>
-      <c r="C10" s="6"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="14"/>
-      <c r="C11" s="6"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="14"/>
-      <c r="C12" s="6"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="14"/>
-      <c r="C13" s="6"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="14"/>
-      <c r="C14" s="6"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="14"/>
-      <c r="C15" s="6"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="18"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="14"/>
-      <c r="C16" s="6"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="14"/>
-      <c r="C17" s="6"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="14"/>
-      <c r="C18" s="6"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="18"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="14"/>
-      <c r="C19" s="6"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="18"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="14"/>
-      <c r="C20" s="6"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="14"/>
-      <c r="C21" s="6"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="18"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="14"/>
-      <c r="C22" s="6"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="14"/>
-      <c r="C23" s="6"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="18"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="14"/>
-      <c r="C24" s="6"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="18"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="14"/>
-      <c r="C25" s="6"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="18"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="14"/>
-      <c r="C26" s="6"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="18"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="14"/>
-      <c r="C27" s="6"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="18"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="14"/>
-      <c r="C28" s="6"/>
+      <c r="C28" s="20"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="18"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="14"/>
-      <c r="C29" s="6"/>
+      <c r="C29" s="20"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="18"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="14"/>
-      <c r="C30" s="6"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="18"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="14"/>
-      <c r="C31" s="6"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="18"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="14"/>
-      <c r="C32" s="6"/>
+      <c r="C32" s="20"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C4:C32" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D4:D32" type="list">
       <formula1>"Nonprofit/NGO,Foundation/Philanthropist,Government/Public Sector/Public Bank,For-profit,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8433,7 +8539,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -8442,53 +8548,56 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.77"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="28.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="D2" s="4"/>
+      <c r="A2" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>260</v>
+      </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="J2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4" t="s">
+        <v>261</v>
+      </c>
       <c r="K2" s="4"/>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="4"/>
+      <c r="M2" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="M2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>248</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>261</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>262</v>
@@ -8506,7 +8615,7 @@
         <v>266</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>262</v>
@@ -8514,57 +8623,63 @@
       <c r="K3" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="M3" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="129.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="B4" s="6" t="s">
         <v>268</v>
       </c>
+      <c r="B4" s="20" t="s">
+        <v>269</v>
+      </c>
       <c r="C4" s="6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="L4" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>279</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14"/>
-      <c r="B5" s="6"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -8574,12 +8689,13 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14"/>
-      <c r="B6" s="6"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -8589,12 +8705,13 @@
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14"/>
-      <c r="B7" s="6"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -8604,12 +8721,13 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="14"/>
-      <c r="B8" s="6"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -8619,12 +8737,13 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14"/>
-      <c r="B9" s="6"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -8634,12 +8753,13 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14"/>
-      <c r="B10" s="6"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -8649,12 +8769,13 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14"/>
-      <c r="B11" s="6"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -8664,12 +8785,13 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14"/>
-      <c r="B12" s="6"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -8679,12 +8801,13 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="14"/>
-      <c r="B13" s="6"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -8694,12 +8817,13 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14"/>
-      <c r="B14" s="6"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -8709,12 +8833,13 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="14"/>
-      <c r="B15" s="6"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -8724,12 +8849,13 @@
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="14"/>
-      <c r="B16" s="6"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -8739,12 +8865,13 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="14"/>
-      <c r="B17" s="6"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -8754,12 +8881,13 @@
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="14"/>
-      <c r="B18" s="6"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -8769,12 +8897,13 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="14"/>
-      <c r="B19" s="6"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -8784,12 +8913,13 @@
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="14"/>
-      <c r="B20" s="6"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -8799,12 +8929,13 @@
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14"/>
-      <c r="B21" s="6"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -8814,12 +8945,13 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14"/>
-      <c r="B22" s="6"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -8829,12 +8961,13 @@
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14"/>
-      <c r="B23" s="6"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -8844,12 +8977,13 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="14"/>
-      <c r="B24" s="6"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -8859,12 +8993,13 @@
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="14"/>
-      <c r="B25" s="6"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -8874,12 +9009,13 @@
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="14"/>
-      <c r="B26" s="6"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -8889,12 +9025,13 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="14"/>
-      <c r="B27" s="6"/>
+      <c r="B27" s="20"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -8904,12 +9041,13 @@
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="14"/>
-      <c r="B28" s="6"/>
+      <c r="B28" s="20"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -8919,12 +9057,13 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="14"/>
-      <c r="B29" s="6"/>
+      <c r="B29" s="20"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -8934,12 +9073,13 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="14"/>
-      <c r="B30" s="6"/>
+      <c r="B30" s="20"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -8949,12 +9089,13 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="14"/>
-      <c r="B31" s="6"/>
+      <c r="B31" s="20"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -8964,12 +9105,13 @@
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="14"/>
-      <c r="B32" s="6"/>
+      <c r="B32" s="20"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -8979,21 +9121,22 @@
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B4:B32" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C4:C32" type="list">
       <formula1>"Nonprofit/NGO,Foundation/Philanthropist,Government/Public Sector/Public Bank,Multilateral/Bilateral/Intergovernmental Financial Institution,Corporate Giving,Investment Fund,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F4:F32" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G4:G32" type="list">
       <formula1>"Interim,Overall"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9013,7 +9156,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -9023,171 +9166,180 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="22.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="M1" s="11"/>
       <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="11"/>
-      <c r="K2" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="L2" s="11"/>
-      <c r="N2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="L2" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="M2" s="11"/>
       <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="15"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="E3" s="4"/>
+      <c r="B3" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>283</v>
+      </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="L3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4" t="s">
+        <v>284</v>
+      </c>
       <c r="M3" s="4"/>
-      <c r="N3" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4" t="s">
+      <c r="N3" s="4"/>
+      <c r="O3" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="Q3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>261</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>284</v>
+        <v>262</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="L4" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="P4" s="13" t="s">
+      <c r="O4" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q4" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="s">
-        <v>295</v>
+    <row r="5" customFormat="false" ht="115.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="19" t="s">
+        <v>297</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>297</v>
+        <v>298</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>299</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="P5" s="14" t="s">
-        <v>310</v>
-      </c>
-      <c r="Q5" s="6" t="s">
         <v>311</v>
       </c>
+      <c r="P5" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q5" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="14"/>
-      <c r="C6" s="6"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -9200,13 +9352,14 @@
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="6"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -9219,13 +9372,14 @@
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="6"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -9238,13 +9392,14 @@
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -9257,13 +9412,14 @@
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="14"/>
-      <c r="C10" s="6"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -9276,13 +9432,14 @@
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="14"/>
-      <c r="C11" s="6"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -9295,13 +9452,14 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="14"/>
-      <c r="C12" s="6"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -9314,13 +9472,14 @@
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="14"/>
-      <c r="C13" s="6"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -9333,13 +9492,14 @@
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="14"/>
-      <c r="C14" s="6"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -9352,13 +9512,14 @@
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="14"/>
-      <c r="C15" s="6"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -9371,13 +9532,14 @@
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="18"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="14"/>
-      <c r="C16" s="6"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -9390,13 +9552,14 @@
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="14"/>
-      <c r="C17" s="6"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -9409,13 +9572,14 @@
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="14"/>
-      <c r="C18" s="6"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -9428,13 +9592,14 @@
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="18"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="14"/>
-      <c r="C19" s="6"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -9447,13 +9612,14 @@
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="18"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="14"/>
-      <c r="C20" s="6"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -9466,13 +9632,14 @@
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="14"/>
-      <c r="C21" s="6"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -9485,13 +9652,14 @@
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="18"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="14"/>
-      <c r="C22" s="6"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -9504,13 +9672,14 @@
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="14"/>
-      <c r="C23" s="6"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -9523,13 +9692,14 @@
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="18"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="14"/>
-      <c r="C24" s="6"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -9542,13 +9712,14 @@
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="18"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="14"/>
-      <c r="C25" s="6"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -9561,13 +9732,14 @@
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="18"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="14"/>
-      <c r="C26" s="6"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
@@ -9580,13 +9752,14 @@
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="18"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="14"/>
-      <c r="C27" s="6"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
@@ -9599,13 +9772,14 @@
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="18"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="14"/>
-      <c r="C28" s="6"/>
+      <c r="C28" s="20"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -9618,13 +9792,14 @@
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="18"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="14"/>
-      <c r="C29" s="6"/>
+      <c r="C29" s="20"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -9637,13 +9812,14 @@
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="18"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="14"/>
-      <c r="C30" s="6"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
@@ -9656,13 +9832,14 @@
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="18"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="14"/>
-      <c r="C31" s="6"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -9675,13 +9852,14 @@
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="18"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="14"/>
-      <c r="C32" s="6"/>
+      <c r="C32" s="20"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
@@ -9694,13 +9872,14 @@
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="18"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="14"/>
-      <c r="C33" s="6"/>
+      <c r="C33" s="20"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
@@ -9713,30 +9892,31 @@
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L5:L33" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M5:M33" type="list">
       <formula1>"IRR,Average annual return"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N5:N33" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O5:O33" type="list">
       <formula1>"No repayment (no principle or return),Some repayment (but below value of principle),Principal repaid (but no net return),Principal + positive financial returns,Not publicly available"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O5:O33" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P5:P33" type="list">
       <formula1>"Debt,Equity,Combination"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C5:C33" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:D33" type="list">
       <formula1>InvestmentsOrgRoleOptions!$A$1:$A$9</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
pipeline: Simplify some enum options
Add code to map old data
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/pipeline_public_v001.xlsx
+++ b/indigo/spreadsheetform_guides/pipeline_public_v001.xlsx
@@ -6514,10 +6514,6 @@
       <formula1>"Current,Abandoned,Launched"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C17" type="list">
-      <formula1>"Scoping (e.g. pre-feasibility study to support market mapping and issue identification),Early stage (e.g. beginning a feasibility study),Late stage (e.g. final deal construction and placement),Final negotiations"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C40" type="list">
       <formula1>"Q1 - 2022,Q2 - 2022,Q3 - 2022,Q4 - 2022,Q1 - 2023,Q2 - 2023,Don’t Know"</formula1>
       <formula2>0</formula2>
@@ -6528,6 +6524,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C130:C133" type="list">
       <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C17" type="list">
+      <formula1>"Scoping,Early stage,Late stage,Final negotiations"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>